<commit_message>
feat & refactor: CRS
Renamed the CRS test class to be more generic and include all CRS
description methods as seperate classes.

Addded tests for name and wkid.
</commit_message>
<xml_diff>
--- a/fc_profiler_requirements.xlsx
+++ b/fc_profiler_requirements.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_4EDCAA32C41C9482C02F21006E8EA814C74780C6" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{AC6D6EFC-6CEE-488E-B7F6-7A3EFF6D062E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>status</t>
   </si>
@@ -46,15 +47,9 @@
     <t>priority</t>
   </si>
   <si>
-    <t>return the CRS of the input FC or NONE</t>
-  </si>
-  <si>
     <t>get_crs_type</t>
   </si>
   <si>
-    <t>get_crs_factory_code</t>
-  </si>
-  <si>
     <t>returns the coordinate reference system factory code (EPSG/WKID)</t>
   </si>
   <si>
@@ -89,12 +84,21 @@
   </si>
   <si>
     <t>get_row_count</t>
+  </si>
+  <si>
+    <t>get_crs_wkid</t>
+  </si>
+  <si>
+    <t>return the CRS name</t>
+  </si>
+  <si>
+    <t>return the CRS or NONE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,10 +163,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="status" displayName="status" ref="A1:A4" totalsRowShown="0">
-  <autoFilter ref="A1:A4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="status" displayName="status" ref="A1:A4" totalsRowShown="0">
+  <autoFilter ref="A1:A4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="status"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -430,12 +434,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +458,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -471,10 +475,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -485,10 +489,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -499,16 +503,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -516,16 +520,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -533,13 +537,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -547,10 +554,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -561,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
@@ -575,21 +582,21 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT("Status[status]")</formula1>
     </dataValidation>
   </dataValidations>
@@ -599,7 +606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>